<commit_message>
Bug fix Out of Range
z.190
</commit_message>
<xml_diff>
--- a/Daten.xlsx
+++ b/Daten.xlsx
@@ -1179,7 +1179,7 @@
         </is>
       </c>
       <c r="W12" s="5" t="n">
-        <v>12171</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="13">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="W13" s="5" t="n">
-        <v>3269</v>
+        <v>591</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" thickBot="1">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="W14" s="7" t="n">
-        <v>1410</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" thickBot="1"/>
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="W18" s="5" t="n">
-        <v>14944</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="19">
@@ -1596,7 +1596,7 @@
         </is>
       </c>
       <c r="W19" s="5" t="n">
-        <v>7032</v>
+        <v>550</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" thickBot="1">
@@ -1666,7 +1666,7 @@
         </is>
       </c>
       <c r="W20" s="7" t="n">
-        <v>4381</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" thickBot="1"/>
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="W24" s="5" t="n">
-        <v>28261</v>
+        <v>15128</v>
       </c>
     </row>
     <row r="25">
@@ -1887,7 +1887,7 @@
         </is>
       </c>
       <c r="W25" s="5" t="n">
-        <v>11251</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" thickBot="1">
@@ -1947,7 +1947,7 @@
         </is>
       </c>
       <c r="W26" s="7" t="n">
-        <v>10388</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" thickBot="1"/>
@@ -2078,11 +2078,11 @@
       </c>
       <c r="V30" s="4" t="inlineStr">
         <is>
-          <t>Dec21</t>
+          <t>Mar22</t>
         </is>
       </c>
       <c r="W30" s="5" t="n">
-        <v>10</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="31">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="V31" s="4" t="inlineStr">
         <is>
-          <t>Mar22</t>
+          <t>May22</t>
         </is>
       </c>
       <c r="W31" s="5" t="n">
-        <v>9700</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" thickBot="1">
@@ -2178,11 +2178,11 @@
       </c>
       <c r="V32" s="6" t="inlineStr">
         <is>
-          <t>May22</t>
+          <t>Jul22</t>
         </is>
       </c>
       <c r="W32" s="7" t="n">
-        <v>2932</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" thickBot="1"/>
@@ -2265,7 +2265,7 @@
         </is>
       </c>
       <c r="W36" s="5" t="n">
-        <v>978</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="W37" s="5" t="n">
-        <v>1031</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" thickBot="1">
@@ -2325,7 +2325,7 @@
         </is>
       </c>
       <c r="W38" s="7" t="n">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" thickBot="1"/>
@@ -2516,7 +2516,7 @@
         </is>
       </c>
       <c r="B54" s="5" t="n">
-        <v>13484</v>
+        <v>4001</v>
       </c>
     </row>
     <row r="55">
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="B55" s="5" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" thickBot="1">

</xml_diff>

<commit_message>
Bug Fix -> Out of Range
</commit_message>
<xml_diff>
--- a/Daten.xlsx
+++ b/Daten.xlsx
@@ -731,67 +731,67 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>1,318</t>
+          <t>590</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
+          <t>FEB 2022</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>317,628</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>MAR 2022</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>1,322,362</t>
+        </is>
+      </c>
+      <c r="J6" s="4" t="inlineStr">
+        <is>
+          <t>MAR 2022</t>
+        </is>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>349,493</t>
+        </is>
+      </c>
+      <c r="M6" s="4" t="inlineStr">
+        <is>
+          <t>MAR 2022</t>
+        </is>
+      </c>
+      <c r="N6" s="5" t="inlineStr">
+        <is>
+          <t>146,023</t>
+        </is>
+      </c>
+      <c r="P6" s="4" t="inlineStr">
+        <is>
+          <t>DEC 2021</t>
+        </is>
+      </c>
+      <c r="Q6" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S6" s="4" t="inlineStr">
+        <is>
           <t>JAN 2022</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
-        <is>
-          <t>36,727</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr">
-        <is>
-          <t>DEC 2021</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J6" s="4" t="inlineStr">
-        <is>
-          <t>DEC 2021</t>
-        </is>
-      </c>
-      <c r="K6" s="5" t="inlineStr">
-        <is>
-          <t>328</t>
-        </is>
-      </c>
-      <c r="M6" s="4" t="inlineStr">
-        <is>
-          <t>MAR 2022</t>
-        </is>
-      </c>
-      <c r="N6" s="5" t="inlineStr">
-        <is>
-          <t>106,042</t>
-        </is>
-      </c>
-      <c r="P6" s="4" t="inlineStr">
-        <is>
-          <t>DEC 2021</t>
-        </is>
-      </c>
-      <c r="Q6" s="5" t="inlineStr">
-        <is>
-          <t>765</t>
-        </is>
-      </c>
-      <c r="S6" s="4" t="inlineStr">
-        <is>
-          <t>DEC 2021</t>
-        </is>
-      </c>
       <c r="T6" s="5" t="inlineStr">
         <is>
-          <t>226</t>
+          <t>116</t>
         </is>
       </c>
       <c r="V6" s="4" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="W6" s="5" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>99</t>
         </is>
       </c>
     </row>
@@ -813,67 +813,67 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>991</t>
+          <t>426</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
+          <t>MAR 2022</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>112,228</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>JUN 2022</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>768</t>
+        </is>
+      </c>
+      <c r="J7" s="4" t="inlineStr">
+        <is>
+          <t>JUN 2022</t>
+        </is>
+      </c>
+      <c r="K7" s="5" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="M7" s="4" t="inlineStr">
+        <is>
+          <t>MAY 2022</t>
+        </is>
+      </c>
+      <c r="N7" s="5" t="inlineStr">
+        <is>
+          <t>37,391</t>
+        </is>
+      </c>
+      <c r="P7" s="4" t="inlineStr">
+        <is>
           <t>FEB 2022</t>
         </is>
       </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>492,217</t>
-        </is>
-      </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>MAR 2022</t>
-        </is>
-      </c>
-      <c r="H7" s="5" t="inlineStr">
-        <is>
-          <t>2,097,624</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>MAR 2022</t>
-        </is>
-      </c>
-      <c r="K7" s="5" t="inlineStr">
-        <is>
-          <t>320,827</t>
-        </is>
-      </c>
-      <c r="M7" s="4" t="inlineStr">
-        <is>
-          <t>MAY 2022</t>
-        </is>
-      </c>
-      <c r="N7" s="5" t="inlineStr">
-        <is>
-          <t>32,195</t>
-        </is>
-      </c>
-      <c r="P7" s="4" t="inlineStr">
+      <c r="Q7" s="5" t="inlineStr">
+        <is>
+          <t>19,752</t>
+        </is>
+      </c>
+      <c r="S7" s="4" t="inlineStr">
         <is>
           <t>FEB 2022</t>
         </is>
       </c>
-      <c r="Q7" s="5" t="inlineStr">
-        <is>
-          <t>20,294</t>
-        </is>
-      </c>
-      <c r="S7" s="4" t="inlineStr">
-        <is>
-          <t>JAN 2022</t>
-        </is>
-      </c>
       <c r="T7" s="5" t="inlineStr">
         <is>
-          <t>419</t>
+          <t>168,305</t>
         </is>
       </c>
       <c r="V7" s="4" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="W7" s="5" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>255</t>
         </is>
       </c>
     </row>
@@ -895,37 +895,37 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>122,480</t>
+          <t>143,496</t>
         </is>
       </c>
       <c r="D8" s="6" t="inlineStr">
         <is>
-          <t>MAR 2022</t>
+          <t>APR 2022</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>129,078</t>
+          <t>43,359</t>
         </is>
       </c>
       <c r="G8" s="6" t="inlineStr">
         <is>
+          <t>SEP 2022</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="J8" s="6" t="inlineStr">
+        <is>
           <t>JUN 2022</t>
         </is>
       </c>
-      <c r="H8" s="7" t="inlineStr">
-        <is>
-          <t>1,381</t>
-        </is>
-      </c>
-      <c r="J8" s="6" t="inlineStr">
-        <is>
-          <t>JUN 2022</t>
-        </is>
-      </c>
       <c r="K8" s="7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="M8" s="6" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="N8" s="7" t="inlineStr">
         <is>
-          <t>20,538</t>
+          <t>28,396</t>
         </is>
       </c>
       <c r="P8" s="6" t="inlineStr">
@@ -945,17 +945,17 @@
       </c>
       <c r="Q8" s="7" t="inlineStr">
         <is>
-          <t>10,557</t>
+          <t>13,323</t>
         </is>
       </c>
       <c r="S8" s="6" t="inlineStr">
         <is>
-          <t>FEB 2022</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="T8" s="7" t="inlineStr">
         <is>
-          <t>105,386</t>
+          <t>18</t>
         </is>
       </c>
       <c r="V8" s="6" t="inlineStr">
@@ -965,7 +965,7 @@
       </c>
       <c r="W8" s="7" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>20</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>14,222</t>
+          <t>21,619</t>
         </is>
       </c>
       <c r="D12" s="4" t="inlineStr">
@@ -1120,27 +1120,27 @@
       </c>
       <c r="E12" s="5" t="inlineStr">
         <is>
-          <t>43,218</t>
+          <t>30</t>
         </is>
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>DEC 2021</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="H12" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>513,549</t>
         </is>
       </c>
       <c r="J12" s="4" t="inlineStr">
         <is>
-          <t>DEC 2021</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="K12" s="5" t="inlineStr">
         <is>
-          <t>1,598</t>
+          <t>1,428,084</t>
         </is>
       </c>
       <c r="M12" s="4" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="N12" s="5" t="inlineStr">
         <is>
-          <t>38,677</t>
+          <t>42,116</t>
         </is>
       </c>
       <c r="P12" s="4" t="inlineStr">
@@ -1160,17 +1160,17 @@
       </c>
       <c r="Q12" s="5" t="inlineStr">
         <is>
-          <t>3,054</t>
+          <t>926</t>
         </is>
       </c>
       <c r="S12" s="4" t="inlineStr">
         <is>
-          <t>DEC 2021</t>
+          <t>JAN 2022</t>
         </is>
       </c>
       <c r="T12" s="5" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>31</t>
         </is>
       </c>
       <c r="V12" s="4" t="inlineStr">
@@ -1179,7 +1179,7 @@
         </is>
       </c>
       <c r="W12" s="5" t="n">
-        <v>5696</v>
+        <v>8719</v>
       </c>
     </row>
     <row r="13">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D13" s="4" t="inlineStr">
@@ -1200,27 +1200,27 @@
       </c>
       <c r="E13" s="5" t="inlineStr">
         <is>
-          <t>59,717</t>
+          <t>50,467</t>
         </is>
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>MAR 2022</t>
+          <t>JUN 2022</t>
         </is>
       </c>
       <c r="H13" s="5" t="inlineStr">
         <is>
-          <t>676,197</t>
+          <t>717</t>
         </is>
       </c>
       <c r="J13" s="4" t="inlineStr">
         <is>
-          <t>MAR 2022</t>
+          <t>JUN 2022</t>
         </is>
       </c>
       <c r="K13" s="5" t="inlineStr">
         <is>
-          <t>1,215,343</t>
+          <t>41</t>
         </is>
       </c>
       <c r="M13" s="4" t="inlineStr">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="N13" s="5" t="inlineStr">
         <is>
-          <t>11,679</t>
+          <t>9,052</t>
         </is>
       </c>
       <c r="P13" s="4" t="inlineStr">
@@ -1240,17 +1240,17 @@
       </c>
       <c r="Q13" s="5" t="inlineStr">
         <is>
-          <t>4,059</t>
+          <t>5,042</t>
         </is>
       </c>
       <c r="S13" s="4" t="inlineStr">
         <is>
-          <t>JAN 2022</t>
+          <t>FEB 2022</t>
         </is>
       </c>
       <c r="T13" s="5" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>346</t>
         </is>
       </c>
       <c r="V13" s="4" t="inlineStr">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="W13" s="5" t="n">
-        <v>1794</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" thickBot="1">
@@ -1280,27 +1280,27 @@
       </c>
       <c r="E14" s="7" t="inlineStr">
         <is>
-          <t>27,404</t>
+          <t>27,309</t>
         </is>
       </c>
       <c r="G14" s="6" t="inlineStr">
         <is>
+          <t>SEP 2022</t>
+        </is>
+      </c>
+      <c r="H14" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J14" s="6" t="inlineStr">
+        <is>
           <t>JUN 2022</t>
         </is>
       </c>
-      <c r="H14" s="7" t="inlineStr">
-        <is>
-          <t>870</t>
-        </is>
-      </c>
-      <c r="J14" s="6" t="inlineStr">
-        <is>
-          <t>JUN 2022</t>
-        </is>
-      </c>
       <c r="K14" s="7" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>8</t>
         </is>
       </c>
       <c r="M14" s="6" t="inlineStr">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="N14" s="7" t="inlineStr">
         <is>
-          <t>7,373</t>
+          <t>9,109</t>
         </is>
       </c>
       <c r="P14" s="6" t="inlineStr">
@@ -1320,17 +1320,17 @@
       </c>
       <c r="Q14" s="7" t="inlineStr">
         <is>
-          <t>1,253</t>
+          <t>1,665</t>
         </is>
       </c>
       <c r="S14" s="6" t="inlineStr">
         <is>
-          <t>FEB 2022</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="T14" s="7" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>46,323</t>
         </is>
       </c>
       <c r="V14" s="6" t="inlineStr">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="W14" s="7" t="n">
-        <v>642</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" thickBot="1"/>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>24</t>
         </is>
       </c>
       <c r="D18" s="4" t="inlineStr">
@@ -1477,17 +1477,17 @@
       </c>
       <c r="E18" s="5" t="inlineStr">
         <is>
-          <t>47,739</t>
+          <t>90</t>
         </is>
       </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
-          <t>DEC 2021</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="H18" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>158,894</t>
         </is>
       </c>
       <c r="M18" s="4" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="N18" s="5" t="inlineStr">
         <is>
-          <t>856</t>
+          <t>275</t>
         </is>
       </c>
       <c r="P18" s="4" t="inlineStr">
@@ -1507,17 +1507,17 @@
       </c>
       <c r="Q18" s="5" t="inlineStr">
         <is>
-          <t>12,992</t>
+          <t>12,432</t>
         </is>
       </c>
       <c r="S18" s="4" t="inlineStr">
         <is>
-          <t>DEC 2021</t>
+          <t>JAN 2022</t>
         </is>
       </c>
       <c r="T18" s="5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>231</t>
         </is>
       </c>
       <c r="V18" s="4" t="inlineStr">
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="W18" s="5" t="n">
-        <v>10003</v>
+        <v>7716</v>
       </c>
     </row>
     <row r="19">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>16</t>
         </is>
       </c>
       <c r="D19" s="4" t="inlineStr">
@@ -1547,17 +1547,17 @@
       </c>
       <c r="E19" s="5" t="inlineStr">
         <is>
-          <t>50,444</t>
+          <t>51,351</t>
         </is>
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>MAR 2022</t>
+          <t>JUN 2022</t>
         </is>
       </c>
       <c r="H19" s="5" t="inlineStr">
         <is>
-          <t>220,121</t>
+          <t>40</t>
         </is>
       </c>
       <c r="M19" s="4" t="inlineStr">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="N19" s="5" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>13</t>
         </is>
       </c>
       <c r="P19" s="4" t="inlineStr">
@@ -1577,17 +1577,17 @@
       </c>
       <c r="Q19" s="5" t="inlineStr">
         <is>
-          <t>5,131</t>
+          <t>6,628</t>
         </is>
       </c>
       <c r="S19" s="4" t="inlineStr">
         <is>
-          <t>JAN 2022</t>
+          <t>FEB 2022</t>
         </is>
       </c>
       <c r="T19" s="5" t="inlineStr">
         <is>
-          <t>18,484</t>
+          <t>21</t>
         </is>
       </c>
       <c r="V19" s="4" t="inlineStr">
@@ -1596,7 +1596,7 @@
         </is>
       </c>
       <c r="W19" s="5" t="n">
-        <v>5003</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" thickBot="1">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="B20" s="7" t="inlineStr">
         <is>
-          <t>81,993</t>
+          <t>68,537</t>
         </is>
       </c>
       <c r="D20" s="6" t="inlineStr">
@@ -1617,17 +1617,17 @@
       </c>
       <c r="E20" s="7" t="inlineStr">
         <is>
-          <t>21,256</t>
+          <t>24,133</t>
         </is>
       </c>
       <c r="G20" s="6" t="inlineStr">
         <is>
-          <t>JUN 2022</t>
+          <t>SEP 2022</t>
         </is>
       </c>
       <c r="H20" s="7" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M20" s="6" t="inlineStr">
@@ -1637,7 +1637,7 @@
       </c>
       <c r="N20" s="7" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>7</t>
         </is>
       </c>
       <c r="P20" s="6" t="inlineStr">
@@ -1647,17 +1647,17 @@
       </c>
       <c r="Q20" s="7" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>152</t>
         </is>
       </c>
       <c r="S20" s="6" t="inlineStr">
         <is>
-          <t>FEB 2022</t>
+          <t>APR 2022</t>
         </is>
       </c>
       <c r="T20" s="7" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>18,494</t>
         </is>
       </c>
       <c r="V20" s="6" t="inlineStr">
@@ -1666,7 +1666,7 @@
         </is>
       </c>
       <c r="W20" s="7" t="n">
-        <v>3190</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" thickBot="1"/>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>63</t>
         </is>
       </c>
       <c r="D24" s="4" t="inlineStr">
@@ -1788,37 +1788,37 @@
       </c>
       <c r="E24" s="5" t="inlineStr">
         <is>
-          <t>47,739</t>
+          <t>90</t>
         </is>
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>DEC 2021</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="H24" s="5" t="inlineStr">
         <is>
+          <t>222,614</t>
+        </is>
+      </c>
+      <c r="M24" s="4" t="inlineStr">
+        <is>
+          <t>JAN 2022</t>
+        </is>
+      </c>
+      <c r="N24" s="5" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="M24" s="4" t="inlineStr">
-        <is>
-          <t>JAN 2022</t>
-        </is>
-      </c>
-      <c r="N24" s="5" t="inlineStr">
-        <is>
-          <t>499</t>
-        </is>
-      </c>
       <c r="S24" s="4" t="inlineStr">
         <is>
-          <t>DEC 2021</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="T24" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1,225</t>
         </is>
       </c>
       <c r="V24" s="4" t="inlineStr">
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="W24" s="5" t="n">
-        <v>28908</v>
+        <v>19027</v>
       </c>
     </row>
     <row r="25">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="B25" s="5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>48</t>
         </is>
       </c>
       <c r="D25" s="4" t="inlineStr">
@@ -1848,17 +1848,17 @@
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>50,444</t>
+          <t>51,351</t>
         </is>
       </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>MAR 2022</t>
+          <t>JUN 2022</t>
         </is>
       </c>
       <c r="H25" s="5" t="inlineStr">
         <is>
-          <t>292,340</t>
+          <t>95</t>
         </is>
       </c>
       <c r="M25" s="4" t="inlineStr">
@@ -1868,17 +1868,17 @@
       </c>
       <c r="N25" s="5" t="inlineStr">
         <is>
-          <t>548</t>
+          <t>584</t>
         </is>
       </c>
       <c r="S25" s="4" t="inlineStr">
         <is>
-          <t>JAN 2022</t>
+          <t>JUN 2022</t>
         </is>
       </c>
       <c r="T25" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>16</t>
         </is>
       </c>
       <c r="V25" s="4" t="inlineStr">
@@ -1887,7 +1887,7 @@
         </is>
       </c>
       <c r="W25" s="5" t="n">
-        <v>10733</v>
+        <v>6927</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" thickBot="1">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="B26" s="7" t="inlineStr">
         <is>
-          <t>74,521</t>
+          <t>59,070</t>
         </is>
       </c>
       <c r="D26" s="6" t="inlineStr">
@@ -1908,17 +1908,17 @@
       </c>
       <c r="E26" s="7" t="inlineStr">
         <is>
-          <t>21,256</t>
+          <t>24,133</t>
         </is>
       </c>
       <c r="G26" s="6" t="inlineStr">
         <is>
-          <t>JUN 2022</t>
+          <t>SEP 2022</t>
         </is>
       </c>
       <c r="H26" s="7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M26" s="6" t="inlineStr">
@@ -1928,12 +1928,12 @@
       </c>
       <c r="N26" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>28</t>
         </is>
       </c>
       <c r="S26" s="6" t="inlineStr">
         <is>
-          <t>FEB 2022</t>
+          <t>SEP 2022</t>
         </is>
       </c>
       <c r="T26" s="7" t="inlineStr">
@@ -1947,7 +1947,7 @@
         </is>
       </c>
       <c r="W26" s="7" t="n">
-        <v>10178</v>
+        <v>5315</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" thickBot="1"/>
@@ -2043,37 +2043,37 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>19,935</t>
+          <t>15,411</t>
         </is>
       </c>
       <c r="D30" s="4" t="inlineStr">
         <is>
+          <t>FEB 2022</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="inlineStr">
+        <is>
+          <t>99,069</t>
+        </is>
+      </c>
+      <c r="M30" s="4" t="inlineStr">
+        <is>
           <t>JAN 2022</t>
         </is>
       </c>
-      <c r="E30" s="5" t="inlineStr">
-        <is>
-          <t>128,582</t>
-        </is>
-      </c>
-      <c r="M30" s="4" t="inlineStr">
+      <c r="N30" s="5" t="inlineStr">
+        <is>
+          <t>3,434</t>
+        </is>
+      </c>
+      <c r="S30" s="4" t="inlineStr">
         <is>
           <t>JAN 2022</t>
         </is>
       </c>
-      <c r="N30" s="5" t="inlineStr">
-        <is>
-          <t>83,928</t>
-        </is>
-      </c>
-      <c r="S30" s="4" t="inlineStr">
-        <is>
-          <t>DEC 2021</t>
-        </is>
-      </c>
       <c r="T30" s="5" t="inlineStr">
         <is>
-          <t>490</t>
+          <t>544</t>
         </is>
       </c>
       <c r="V30" s="4" t="inlineStr">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="W30" s="5" t="n">
-        <v>10605</v>
+        <v>9452</v>
       </c>
     </row>
     <row r="31">
@@ -2093,37 +2093,37 @@
       </c>
       <c r="B31" s="5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D31" s="4" t="inlineStr">
         <is>
+          <t>MAR 2022</t>
+        </is>
+      </c>
+      <c r="E31" s="5" t="inlineStr">
+        <is>
+          <t>52,865</t>
+        </is>
+      </c>
+      <c r="M31" s="4" t="inlineStr">
+        <is>
+          <t>MAR 2022</t>
+        </is>
+      </c>
+      <c r="N31" s="5" t="inlineStr">
+        <is>
+          <t>90,234</t>
+        </is>
+      </c>
+      <c r="S31" s="4" t="inlineStr">
+        <is>
           <t>FEB 2022</t>
         </is>
       </c>
-      <c r="E31" s="5" t="inlineStr">
-        <is>
-          <t>61,251</t>
-        </is>
-      </c>
-      <c r="M31" s="4" t="inlineStr">
-        <is>
-          <t>MAR 2022</t>
-        </is>
-      </c>
-      <c r="N31" s="5" t="inlineStr">
-        <is>
-          <t>70,137</t>
-        </is>
-      </c>
-      <c r="S31" s="4" t="inlineStr">
-        <is>
-          <t>JAN 2022</t>
-        </is>
-      </c>
       <c r="T31" s="5" t="inlineStr">
         <is>
-          <t>438</t>
+          <t>242</t>
         </is>
       </c>
       <c r="V31" s="4" t="inlineStr">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="W31" s="5" t="n">
-        <v>4162</v>
+        <v>3016</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" thickBot="1">
@@ -2148,12 +2148,12 @@
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
-          <t>MAR 2022</t>
+          <t>APR 2022</t>
         </is>
       </c>
       <c r="E32" s="7" t="inlineStr">
         <is>
-          <t>49,456</t>
+          <t>33,114</t>
         </is>
       </c>
       <c r="M32" s="6" t="inlineStr">
@@ -2163,17 +2163,17 @@
       </c>
       <c r="N32" s="7" t="inlineStr">
         <is>
-          <t>22,449</t>
+          <t>23,632</t>
         </is>
       </c>
       <c r="S32" s="6" t="inlineStr">
         <is>
-          <t>FEB 2022</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="T32" s="7" t="inlineStr">
         <is>
-          <t>325</t>
+          <t>38,420</t>
         </is>
       </c>
       <c r="V32" s="6" t="inlineStr">
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="W32" s="7" t="n">
-        <v>1979</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" thickBot="1"/>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="B36" s="5" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>69</t>
         </is>
       </c>
       <c r="M36" s="4" t="inlineStr">
@@ -2256,7 +2256,7 @@
       </c>
       <c r="N36" s="5" t="inlineStr">
         <is>
-          <t>27,642</t>
+          <t>518</t>
         </is>
       </c>
       <c r="V36" s="4" t="inlineStr">
@@ -2265,7 +2265,7 @@
         </is>
       </c>
       <c r="W36" s="5" t="n">
-        <v>303</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B37" s="5" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>744</t>
         </is>
       </c>
       <c r="M37" s="4" t="inlineStr">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="N37" s="5" t="inlineStr">
         <is>
-          <t>33,428</t>
+          <t>34,226</t>
         </is>
       </c>
       <c r="V37" s="4" t="inlineStr">
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="W37" s="5" t="n">
-        <v>453</v>
+        <v>315</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" thickBot="1">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="B38" s="7" t="inlineStr">
         <is>
-          <t>70,614</t>
+          <t>50,466</t>
         </is>
       </c>
       <c r="M38" s="6" t="inlineStr">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="N38" s="7" t="inlineStr">
         <is>
-          <t>9,765</t>
+          <t>13,249</t>
         </is>
       </c>
       <c r="V38" s="6" t="inlineStr">
@@ -2325,7 +2325,7 @@
         </is>
       </c>
       <c r="W38" s="7" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" thickBot="1"/>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="B42" s="5" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>27</t>
         </is>
       </c>
       <c r="M42" s="4" t="inlineStr">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="N42" s="5" t="inlineStr">
         <is>
-          <t>29,815</t>
+          <t>587</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="B43" s="5" t="inlineStr">
         <is>
-          <t>1,855</t>
+          <t>324</t>
         </is>
       </c>
       <c r="M43" s="4" t="inlineStr">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="N43" s="5" t="inlineStr">
         <is>
-          <t>35,529</t>
+          <t>58,814</t>
         </is>
       </c>
     </row>
@@ -2417,7 +2417,7 @@
       </c>
       <c r="B44" s="7" t="inlineStr">
         <is>
-          <t>79,458</t>
+          <t>79,656</t>
         </is>
       </c>
       <c r="M44" s="6" t="inlineStr">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="N44" s="7" t="inlineStr">
         <is>
-          <t>10,976</t>
+          <t>20,266</t>
         </is>
       </c>
     </row>
@@ -2460,31 +2460,31 @@
       </c>
       <c r="B48" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>MAR 2022</t>
+          <t>FEB 2022</t>
         </is>
       </c>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>36,547</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" thickBot="1">
       <c r="A50" s="6" t="inlineStr">
         <is>
-          <t>JUN 2022</t>
+          <t>MAR 2022</t>
         </is>
       </c>
       <c r="B50" s="7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>31,843</t>
         </is>
       </c>
     </row>
@@ -2516,7 +2516,7 @@
         </is>
       </c>
       <c r="B54" s="5" t="n">
-        <v>8665</v>
+        <v>7453</v>
       </c>
     </row>
     <row r="55">
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="B55" s="5" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" thickBot="1">

</xml_diff>